<commit_message>
add functionality to insert all collections from excel on start
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\JavaScript\excel-to-json\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Documents\Code\JavaScript\excel-to-mongo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3307C404-49D1-4EDE-B3E2-66A0F4A52D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C194E59-A588-4DB3-8CBC-B85A09E3CED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="34125" windowHeight="13275" xr2:uid="{DBCDF870-5942-4714-9E89-13B949365442}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DBCDF870-5942-4714-9E89-13B949365442}"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="1" r:id="rId1"/>
@@ -32,18 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>title</t>
   </si>
   <si>
     <t>author</t>
-  </si>
-  <si>
-    <t>series</t>
-  </si>
-  <si>
-    <t>numInSeries</t>
   </si>
   <si>
     <t>isRead</t>
@@ -428,18 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CA693C-629C-474E-A124-01DBBF70FE0E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,112 +440,70 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="b">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
+      <c r="C7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>